<commit_message>
Fixing UnoInlineUAV and TiltieTailed for post hackathon submission
</commit_message>
<xml_diff>
--- a/designs-hackathon2/_Summary.xlsx
+++ b/designs-hackathon2/_Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\symbench\athens-graphops\designs-hackathon2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530EE147-625B-4829-9754-340E22B4385D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4A7BFC-1D61-4609-8F81-8D7939740F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="16200" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>Design</t>
   </si>
@@ -131,9 +131,6 @@
     <t>InlineUAV</t>
   </si>
   <si>
-    <t>NO STUDY PARAMS</t>
-  </si>
-  <si>
     <t>first 8 prop design</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
   </si>
   <si>
     <t>Tiltie</t>
-  </si>
-  <si>
-    <t>ONLY ONE PROP IS ROTATED</t>
   </si>
   <si>
     <t>tilted props, single wing, inline cargo</t>
@@ -216,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,8 +229,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -259,32 +259,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -300,12 +274,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,14 +606,14 @@
         <v>15</v>
       </c>
       <c r="N1" s="5"/>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S1">
         <v>1926</v>
@@ -684,10 +654,10 @@
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
       <c r="R2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S2">
         <v>0.8</v>
@@ -707,7 +677,7 @@
         <v>2751</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E17" si="0">SUM(C3:D3) * IF(AND(C3&gt;$S$1, D3&gt;$S$1, H3 &lt; $S$2), 1.5, 1)</f>
+        <f>SUM(C3:D3) * IF(AND(C3&gt;$S$1, D3&gt;$S$1, H3 &lt; $S$2), 1.5, 1)</f>
         <v>8271</v>
       </c>
       <c r="F3" s="4">
@@ -717,7 +687,7 @@
         <v>0.186720416</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H13" si="1">SUM(F3:G3)</f>
+        <f>SUM(F3:G3)</f>
         <v>0.37651315299999999</v>
       </c>
       <c r="I3" s="4">
@@ -759,7 +729,7 @@
         <v>2746</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C4:D4) * IF(AND(C4&gt;$S$1, D4&gt;$S$1, H4 &lt; $S$2), 1.5, 1)</f>
         <v>8254.5</v>
       </c>
       <c r="F4" s="4">
@@ -769,7 +739,7 @@
         <v>0.28607782700000001</v>
       </c>
       <c r="H4" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(F4:G4)</f>
         <v>0.58927160499999998</v>
       </c>
       <c r="I4" s="4">
@@ -811,7 +781,7 @@
         <v>2735</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C5:D5) * IF(AND(C5&gt;$S$1, D5&gt;$S$1, H5 &lt; $S$2), 1.5, 1)</f>
         <v>8214</v>
       </c>
       <c r="F5" s="4">
@@ -821,7 +791,7 @@
         <v>0.169917971</v>
       </c>
       <c r="H5" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(F5:G5)</f>
         <v>0.33726431400000001</v>
       </c>
       <c r="I5" s="4">
@@ -863,7 +833,7 @@
         <v>2721</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C6:D6) * IF(AND(C6&gt;$S$1, D6&gt;$S$1, H6 &lt; $S$2), 1.5, 1)</f>
         <v>8172</v>
       </c>
       <c r="F6" s="4">
@@ -873,7 +843,7 @@
         <v>0.25841948399999998</v>
       </c>
       <c r="H6" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(F6:G6)</f>
         <v>0.519799173</v>
       </c>
       <c r="I6" s="4">
@@ -913,7 +883,7 @@
         <v>2643</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C7:D7) * IF(AND(C7&gt;$S$1, D7&gt;$S$1, H7 &lt; $S$2), 1.5, 1)</f>
         <v>7939.5</v>
       </c>
       <c r="F7" s="4">
@@ -923,7 +893,7 @@
         <v>0.287357837</v>
       </c>
       <c r="H7" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(F7:G7)</f>
         <v>0.55273684899999997</v>
       </c>
       <c r="I7" s="4">
@@ -961,7 +931,7 @@
         <v>2636</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C8:D8) * IF(AND(C8&gt;$S$1, D8&gt;$S$1, H8 &lt; $S$2), 1.5, 1)</f>
         <v>7908</v>
       </c>
       <c r="F8" s="4">
@@ -971,7 +941,7 @@
         <v>0.36214107299999998</v>
       </c>
       <c r="H8" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(F8:G8)</f>
         <v>0.74956268100000001</v>
       </c>
       <c r="I8" s="4">
@@ -996,137 +966,138 @@
       <c r="P8" s="4"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
+      <c r="A9" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B9" s="4">
         <v>0</v>
       </c>
       <c r="C9" s="4">
-        <v>2560</v>
+        <v>2573</v>
       </c>
       <c r="D9" s="4">
-        <v>2560</v>
+        <v>2616</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="0"/>
-        <v>7680</v>
+        <f>SUM(C9:D9) * IF(AND(C9&gt;$S$1, D9&gt;$S$1, H9 &lt; $S$2), 1.5, 1)</f>
+        <v>7783.5</v>
       </c>
       <c r="F9" s="4">
-        <v>0.41063216299999999</v>
+        <v>0.20627899499999999</v>
       </c>
       <c r="G9" s="4">
-        <v>0.37151172799999999</v>
+        <v>0.18730783500000001</v>
       </c>
       <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.78214389100000004</v>
+        <f>SUM(F9:G9)</f>
+        <v>0.39358683</v>
       </c>
       <c r="I9" s="4">
-        <v>4.9409504354245204</v>
+        <v>4.70529370699089</v>
       </c>
       <c r="J9" s="4">
-        <v>4.4419504354245198</v>
+        <v>4.2062937069908903</v>
       </c>
       <c r="K9" s="4">
         <v>4</v>
       </c>
       <c r="L9" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" s="4">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="N9" s="4">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
+      <c r="P9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="2"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>29</v>
+      <c r="A10" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B10" s="4">
         <v>0</v>
       </c>
       <c r="C10" s="4">
-        <v>2444</v>
+        <v>2567</v>
       </c>
       <c r="D10" s="4">
-        <v>2457</v>
+        <v>2566</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="0"/>
-        <v>4901</v>
+        <f>SUM(C10:D10) * IF(AND(C10&gt;$S$1, D10&gt;$S$1, H10 &lt; $S$2), 1.5, 1)</f>
+        <v>7699.5</v>
       </c>
       <c r="F10" s="4">
-        <v>0.57120358900000001</v>
+        <v>0.39486736099999997</v>
       </c>
       <c r="G10" s="4">
-        <v>0.53909260000000003</v>
+        <v>0.357967168</v>
       </c>
       <c r="H10" s="4">
-        <f t="shared" si="1"/>
-        <v>1.110296189</v>
+        <f>SUM(F10:G10)</f>
+        <v>0.75283452900000003</v>
       </c>
       <c r="I10" s="4">
-        <v>5.1645589009229598</v>
+        <v>4.8542122881461998</v>
       </c>
       <c r="J10" s="4">
-        <v>4.6655589009229601</v>
+        <v>4.3552122881462001</v>
       </c>
       <c r="K10" s="4">
-        <v>8</v>
-      </c>
-      <c r="L10" s="4">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="M10" s="4">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N10" s="4">
-        <v>21</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
       </c>
       <c r="C11" s="4">
-        <v>2395</v>
+        <v>2560</v>
       </c>
       <c r="D11" s="4">
-        <v>2395</v>
+        <v>2560</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>4790</v>
+        <f>SUM(C11:D11) * IF(AND(C11&gt;$S$1, D11&gt;$S$1, H11 &lt; $S$2), 1.5, 1)</f>
+        <v>7680</v>
       </c>
       <c r="F11" s="4">
-        <v>0.526838005</v>
+        <v>0.41063216299999999</v>
       </c>
       <c r="G11" s="4">
-        <v>0.45016360300000002</v>
+        <v>0.37151172799999999</v>
       </c>
       <c r="H11" s="4">
-        <f t="shared" si="1"/>
-        <v>0.97700160800000002</v>
+        <f>SUM(F11:G11)</f>
+        <v>0.78214389100000004</v>
       </c>
       <c r="I11" s="4">
-        <v>4.6883676341283804</v>
+        <v>4.9409504354245204</v>
       </c>
       <c r="J11" s="4">
-        <v>4.1893676341283799</v>
+        <v>4.4419504354245198</v>
       </c>
       <c r="K11" s="4">
         <v>4</v>
@@ -1135,193 +1106,217 @@
         <v>2</v>
       </c>
       <c r="M11" s="4">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="N11" s="4">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B12" s="4">
         <v>0</v>
       </c>
       <c r="C12" s="4">
-        <v>2395</v>
+        <v>2444</v>
       </c>
       <c r="D12" s="4">
-        <v>235</v>
+        <v>2457</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
-        <v>2630</v>
+        <f>SUM(C12:D12) * IF(AND(C12&gt;$S$1, D12&gt;$S$1, H12 &lt; $S$2), 1.5, 1)</f>
+        <v>4901</v>
       </c>
       <c r="F12" s="4">
-        <v>0.50372666099999996</v>
+        <v>0.57120358900000001</v>
       </c>
       <c r="G12" s="4">
-        <v>0.11627172700000001</v>
+        <v>0.53909260000000003</v>
       </c>
       <c r="H12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.61999838799999996</v>
+        <f>SUM(F12:G12)</f>
+        <v>1.110296189</v>
       </c>
       <c r="I12" s="4">
-        <v>4.70529370699089</v>
+        <v>5.1645589009229598</v>
       </c>
       <c r="J12" s="4">
-        <v>4.2062937069908903</v>
+        <v>4.6655589009229601</v>
       </c>
       <c r="K12" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12" s="4">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="N12" s="4">
-        <v>15</v>
-      </c>
-      <c r="O12" s="4"/>
+        <v>21</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="P12" s="4" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>2567</v>
-      </c>
-      <c r="D13">
-        <v>2566</v>
+      <c r="C13" s="4">
+        <v>2395</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2395</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
-        <v>7699.5</v>
-      </c>
-      <c r="F13">
-        <v>0.39486736099999997</v>
-      </c>
-      <c r="G13">
-        <v>0.357967168</v>
+        <f>SUM(C13:D13) * IF(AND(C13&gt;$S$1, D13&gt;$S$1, H13 &lt; $S$2), 1.5, 1)</f>
+        <v>4790</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.526838005</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.45016360300000002</v>
       </c>
       <c r="H13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.75283452900000003</v>
-      </c>
-      <c r="I13">
-        <v>4.8542122881461998</v>
-      </c>
-      <c r="J13">
-        <v>4.3552122881462001</v>
+        <f>SUM(F13:G13)</f>
+        <v>0.97700160800000002</v>
+      </c>
+      <c r="I13" s="4">
+        <v>4.6883676341283804</v>
+      </c>
+      <c r="J13" s="4">
+        <v>4.1893676341283799</v>
       </c>
       <c r="K13" s="4">
         <v>4</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>35</v>
+      <c r="L13" s="4">
+        <v>2</v>
       </c>
       <c r="M13" s="4">
+        <v>17</v>
+      </c>
+      <c r="N13" s="4">
         <v>18</v>
       </c>
-      <c r="N13" s="4">
-        <v>19</v>
-      </c>
       <c r="O13" s="4"/>
-      <c r="P13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q13" s="2"/>
+      <c r="P13" s="4"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="4">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2153</v>
+      </c>
+      <c r="D14" s="4">
+        <v>2158</v>
+      </c>
       <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
+        <f>SUM(C14:D14) * IF(AND(C14&gt;$S$1, D14&gt;$S$1, H14 &lt; $S$2), 1.5, 1)</f>
+        <v>4311</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.64166241899999998</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.56194317299999996</v>
+      </c>
+      <c r="H14" s="4">
+        <f>SUM(F14:G14)</f>
+        <v>1.2036055919999999</v>
+      </c>
+      <c r="I14" s="4">
+        <v>5.2968461286825104</v>
+      </c>
+      <c r="J14" s="4">
+        <v>4.7978461286825098</v>
+      </c>
       <c r="K14" s="4">
         <v>4</v>
       </c>
       <c r="L14" s="4">
-        <v>2</v>
-      </c>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>8</v>
+      </c>
+      <c r="N14" s="4">
+        <v>9</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="P14" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>31</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="Q14" s="2"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>36</v>
+      <c r="A15" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C15:D15) * IF(AND(C15&gt;$S$1, D15&gt;$S$1, H15 &lt; $S$2), 1.5, 1)</f>
         <v>0</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <f>SUM(F15:G15)</f>
+        <v>0</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4">
         <v>4</v>
       </c>
       <c r="L15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C16:D16) * IF(AND(C16&gt;$S$1, D16&gt;$S$1, H16 &lt; $S$2), 1.5, 1)</f>
         <v>0</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="4">
+        <f>SUM(F16:G16)</f>
+        <v>0</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4">
@@ -1334,46 +1329,47 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4">
-        <f t="shared" si="0"/>
+        <f>SUM(C17:D17) * IF(AND(C17&gt;$S$1, D17&gt;$S$1, H17 &lt; $S$2), 1.5, 1)</f>
         <v>0</v>
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <f>SUM(F17:G17)</f>
+        <v>0</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4">
         <v>4</v>
       </c>
       <c r="L17" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="O17" s="4"/>
       <c r="P17" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:P17">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:Q17">
     <sortCondition descending="1" ref="E3:E17"/>
   </sortState>
   <mergeCells count="8">

</xml_diff>